<commit_message>
added missed frames info in .xlsx
</commit_message>
<xml_diff>
--- a/2012 08 29 зняті жести.xlsx
+++ b/2012 08 29 зняті жести.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="13470"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="13470" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="жести" sheetId="2" r:id="rId1"/>
     <sheet name="дактиль" sheetId="3" r:id="rId2"/>
     <sheet name="Речення" sheetId="4" r:id="rId3"/>
     <sheet name="Міміка" sheetId="7" r:id="rId4"/>
+    <sheet name="corrupted_frames" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="282">
   <si>
     <t>Здраствуй (те)</t>
   </si>
@@ -518,9 +519,6 @@
   </si>
   <si>
     <t>Мені цікаво читати про історію України</t>
-  </si>
-  <si>
-    <t>Dactyl, D1, D2</t>
   </si>
   <si>
     <t>далеко</t>
@@ -853,12 +851,84 @@
   <si>
     <t>треба пояснити що це за жести</t>
   </si>
+  <si>
+    <t># gesture ID</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>corrupted_files</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>M5_01</t>
+  </si>
+  <si>
+    <t>RMDL3 and RRNG3 are missed</t>
+  </si>
+  <si>
+    <t>H4_mcraw</t>
+  </si>
+  <si>
+    <t>cropped from 269 up to end</t>
+  </si>
+  <si>
+    <t>M5_01_gest1_sample0</t>
+  </si>
+  <si>
+    <t>M5_01_gest1_sample1</t>
+  </si>
+  <si>
+    <t>M5_01_gest2_sample0</t>
+  </si>
+  <si>
+    <t>M5_01_gest2_sample1</t>
+  </si>
+  <si>
+    <t>M5_01_gest3_sample0</t>
+  </si>
+  <si>
+    <t>M5_01_gest3_sample1</t>
+  </si>
+  <si>
+    <t>RMDL3 and RRNG3 are missed    + RIDX3 is off</t>
+  </si>
+  <si>
+    <t>F4_mcraw</t>
+  </si>
+  <si>
+    <t>frames[1882 --&gt; end]: STRN is off</t>
+  </si>
+  <si>
+    <t>F4_mcraw_gest2_sample0</t>
+  </si>
+  <si>
+    <t>F4_mcraw_gest2_sample1</t>
+  </si>
+  <si>
+    <t>F4_mcraw_gest3_sample0</t>
+  </si>
+  <si>
+    <t>F4_mcraw_gest3_sample1</t>
+  </si>
+  <si>
+    <t>STRN is off</t>
+  </si>
+  <si>
+    <t>M5_01_gest0_sample0</t>
+  </si>
+  <si>
+    <t>M5_01_gest0_sample1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -936,6 +1006,15 @@
       <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1011,7 +1090,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1499,13 +1578,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1664,6 +1753,16 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1691,6 +1790,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1706,6 +1814,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1718,32 +1829,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1770,14 +1887,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1785,23 +1899,29 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный_Лист3" xfId="1"/>
     <cellStyle name="Обычный_Речення" xfId="2"/>
@@ -2170,9 +2290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G134" sqref="G134"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2189,13 +2309,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" thickBot="1">
       <c r="A1" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>128</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>129</v>
@@ -2207,18 +2327,18 @@
         <v>126</v>
       </c>
       <c r="G1" s="62" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="J1" s="113" t="s">
         <v>249</v>
       </c>
-      <c r="K1" s="114"/>
+      <c r="J1" s="123" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" s="124"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="115" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="1">
@@ -2233,18 +2353,18 @@
       <c r="E2" s="13">
         <v>1</v>
       </c>
-      <c r="F2" s="121" t="s">
-        <v>200</v>
-      </c>
-      <c r="G2" s="121">
+      <c r="F2" s="131" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="131">
         <v>4</v>
       </c>
-      <c r="H2" s="120" t="s">
-        <v>251</v>
+      <c r="H2" s="130" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="107"/>
+      <c r="A3" s="116"/>
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -2257,12 +2377,12 @@
       <c r="E3" s="13">
         <v>1</v>
       </c>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="105"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="107"/>
     </row>
     <row r="4" spans="1:11" ht="18">
-      <c r="A4" s="107"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -2275,12 +2395,12 @@
       <c r="E4" s="13">
         <v>1</v>
       </c>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="105"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="107"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" thickBot="1">
-      <c r="A5" s="107"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -2293,12 +2413,12 @@
       <c r="E5" s="13">
         <v>1</v>
       </c>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="105"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="107"/>
     </row>
     <row r="6" spans="1:11" ht="18">
-      <c r="A6" s="107"/>
+      <c r="A6" s="116"/>
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -2311,18 +2431,18 @@
       <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="F6" s="95" t="s">
-        <v>201</v>
-      </c>
-      <c r="G6" s="95">
+      <c r="F6" s="102" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="102">
         <v>4</v>
       </c>
-      <c r="H6" s="105" t="s">
-        <v>252</v>
+      <c r="H6" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="18.75" thickBot="1">
-      <c r="A7" s="107"/>
+      <c r="A7" s="116"/>
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -2335,12 +2455,12 @@
       <c r="E7" s="13">
         <v>2</v>
       </c>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="105"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="107"/>
     </row>
     <row r="8" spans="1:11" ht="18">
-      <c r="A8" s="107"/>
+      <c r="A8" s="116"/>
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -2353,18 +2473,18 @@
       <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="F8" s="95" t="s">
-        <v>202</v>
-      </c>
-      <c r="G8" s="95">
+      <c r="F8" s="102" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8" s="102">
         <v>4</v>
       </c>
-      <c r="H8" s="105" t="s">
-        <v>252</v>
+      <c r="H8" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18">
-      <c r="A9" s="107"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="1">
         <v>8</v>
       </c>
@@ -2377,12 +2497,12 @@
       <c r="E9" s="13">
         <v>1</v>
       </c>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="105"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="107"/>
     </row>
     <row r="10" spans="1:11" ht="18">
-      <c r="A10" s="107"/>
+      <c r="A10" s="116"/>
       <c r="B10" s="1">
         <v>9</v>
       </c>
@@ -2393,12 +2513,12 @@
       <c r="E10" s="13">
         <v>1</v>
       </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="105"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="107"/>
     </row>
     <row r="11" spans="1:11" ht="18.75" thickBot="1">
-      <c r="A11" s="107"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -2411,12 +2531,12 @@
       <c r="E11" s="13">
         <v>1</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="105"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="107"/>
     </row>
     <row r="12" spans="1:11" ht="18">
-      <c r="A12" s="107"/>
+      <c r="A12" s="116"/>
       <c r="B12" s="1">
         <v>11</v>
       </c>
@@ -2429,18 +2549,18 @@
       <c r="E12" s="13">
         <v>1</v>
       </c>
-      <c r="F12" s="95" t="s">
-        <v>203</v>
-      </c>
-      <c r="G12" s="95">
+      <c r="F12" s="102" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" s="102">
         <v>4</v>
       </c>
-      <c r="H12" s="105" t="s">
-        <v>252</v>
+      <c r="H12" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18">
-      <c r="A13" s="107"/>
+      <c r="A13" s="116"/>
       <c r="B13" s="1">
         <v>12</v>
       </c>
@@ -2453,12 +2573,12 @@
       <c r="E13" s="13">
         <v>1</v>
       </c>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="105"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:11" ht="18.75" thickBot="1">
-      <c r="A14" s="107"/>
+      <c r="A14" s="116"/>
       <c r="B14" s="1">
         <v>13</v>
       </c>
@@ -2471,12 +2591,12 @@
       <c r="E14" s="13">
         <v>2</v>
       </c>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="105"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="107"/>
     </row>
     <row r="15" spans="1:11" ht="18">
-      <c r="A15" s="107"/>
+      <c r="A15" s="116"/>
       <c r="B15" s="1">
         <v>14</v>
       </c>
@@ -2489,18 +2609,18 @@
       <c r="E15" s="13">
         <v>1</v>
       </c>
-      <c r="F15" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="G15" s="95">
+      <c r="F15" s="102" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="102">
         <v>4</v>
       </c>
-      <c r="H15" s="105" t="s">
-        <v>252</v>
+      <c r="H15" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="18">
-      <c r="A16" s="107"/>
+      <c r="A16" s="116"/>
       <c r="B16" s="1">
         <v>15</v>
       </c>
@@ -2513,12 +2633,12 @@
       <c r="E16" s="13">
         <v>1</v>
       </c>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="105"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="107"/>
     </row>
     <row r="17" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A17" s="107"/>
+      <c r="A17" s="116"/>
       <c r="B17" s="1">
         <v>16</v>
       </c>
@@ -2531,12 +2651,12 @@
       <c r="E17" s="52">
         <v>2</v>
       </c>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="105"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="107"/>
     </row>
     <row r="18" spans="1:9" ht="18.75" thickTop="1">
-      <c r="A18" s="107"/>
+      <c r="A18" s="116"/>
       <c r="B18" s="64">
         <v>17</v>
       </c>
@@ -2549,18 +2669,18 @@
       <c r="E18" s="63">
         <v>2</v>
       </c>
-      <c r="F18" s="115" t="s">
-        <v>205</v>
-      </c>
-      <c r="G18" s="118">
+      <c r="F18" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="128">
         <v>5</v>
       </c>
-      <c r="H18" s="122" t="s">
-        <v>253</v>
+      <c r="H18" s="120" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18">
-      <c r="A19" s="107"/>
+      <c r="A19" s="116"/>
       <c r="B19" s="64">
         <v>18</v>
       </c>
@@ -2573,12 +2693,12 @@
       <c r="E19" s="63">
         <v>2</v>
       </c>
-      <c r="F19" s="116"/>
-      <c r="G19" s="119"/>
-      <c r="H19" s="122"/>
+      <c r="F19" s="126"/>
+      <c r="G19" s="129"/>
+      <c r="H19" s="120"/>
     </row>
     <row r="20" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A20" s="107"/>
+      <c r="A20" s="116"/>
       <c r="B20" s="1">
         <v>19</v>
       </c>
@@ -2586,18 +2706,18 @@
         <v>18</v>
       </c>
       <c r="D20" s="78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E20" s="79">
         <v>1</v>
       </c>
-      <c r="F20" s="116"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="123"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="67"/>
     </row>
     <row r="21" spans="1:9" ht="18.75" thickTop="1">
-      <c r="A21" s="107"/>
+      <c r="A21" s="116"/>
       <c r="B21" s="1">
         <v>20</v>
       </c>
@@ -2610,18 +2730,18 @@
       <c r="E21" s="66">
         <v>1</v>
       </c>
-      <c r="F21" s="117" t="s">
-        <v>206</v>
-      </c>
-      <c r="G21" s="117">
+      <c r="F21" s="127" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="127">
         <v>3</v>
       </c>
-      <c r="H21" s="124" t="s">
-        <v>252</v>
+      <c r="H21" s="122" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18">
-      <c r="A22" s="107"/>
+      <c r="A22" s="116"/>
       <c r="B22" s="1">
         <v>21</v>
       </c>
@@ -2634,12 +2754,12 @@
       <c r="E22" s="66">
         <v>1</v>
       </c>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="124"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="122"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A23" s="107"/>
+      <c r="A23" s="116"/>
       <c r="B23" s="1">
         <v>22</v>
       </c>
@@ -2652,12 +2772,12 @@
       <c r="E23" s="66">
         <v>1</v>
       </c>
-      <c r="F23" s="117"/>
-      <c r="G23" s="117"/>
-      <c r="H23" s="124"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="122"/>
     </row>
     <row r="24" spans="1:9" ht="18">
-      <c r="A24" s="107"/>
+      <c r="A24" s="116"/>
       <c r="B24" s="1">
         <v>23</v>
       </c>
@@ -2670,18 +2790,18 @@
       <c r="E24" s="68">
         <v>1</v>
       </c>
-      <c r="F24" s="95" t="s">
-        <v>207</v>
-      </c>
-      <c r="G24" s="95">
+      <c r="F24" s="102" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="102">
         <v>3</v>
       </c>
-      <c r="H24" s="105" t="s">
-        <v>252</v>
+      <c r="H24" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18">
-      <c r="A25" s="107"/>
+      <c r="A25" s="116"/>
       <c r="B25" s="1">
         <v>24</v>
       </c>
@@ -2694,12 +2814,12 @@
       <c r="E25" s="13">
         <v>1</v>
       </c>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="105"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="107"/>
     </row>
     <row r="26" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A26" s="107"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="1">
         <v>25</v>
       </c>
@@ -2712,12 +2832,12 @@
       <c r="E26" s="13">
         <v>1</v>
       </c>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="105"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="107"/>
     </row>
     <row r="27" spans="1:9" ht="18">
-      <c r="A27" s="107"/>
+      <c r="A27" s="116"/>
       <c r="B27" s="1">
         <v>26</v>
       </c>
@@ -2730,18 +2850,18 @@
       <c r="E27" s="13">
         <v>2</v>
       </c>
-      <c r="F27" s="95" t="s">
-        <v>208</v>
-      </c>
-      <c r="G27" s="95">
+      <c r="F27" s="102" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="102">
         <v>3</v>
       </c>
-      <c r="H27" s="105" t="s">
-        <v>252</v>
+      <c r="H27" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A28" s="108"/>
+      <c r="A28" s="118"/>
       <c r="B28" s="1">
         <v>27</v>
       </c>
@@ -2754,12 +2874,12 @@
       <c r="E28" s="13">
         <v>1</v>
       </c>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="105"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="107"/>
     </row>
     <row r="29" spans="1:9" ht="18">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="115" t="s">
         <v>140</v>
       </c>
       <c r="B29" s="1">
@@ -2774,18 +2894,18 @@
       <c r="E29" s="13">
         <v>1</v>
       </c>
-      <c r="F29" s="95" t="s">
-        <v>211</v>
-      </c>
-      <c r="G29" s="95">
+      <c r="F29" s="102" t="s">
+        <v>210</v>
+      </c>
+      <c r="G29" s="102">
         <v>4</v>
       </c>
-      <c r="H29" s="105" t="s">
-        <v>252</v>
+      <c r="H29" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="107"/>
+      <c r="A30" s="116"/>
       <c r="B30" s="1">
         <v>29</v>
       </c>
@@ -2798,12 +2918,12 @@
       <c r="E30" s="13">
         <v>1</v>
       </c>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="105"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="107"/>
     </row>
     <row r="31" spans="1:9" ht="18">
-      <c r="A31" s="107"/>
+      <c r="A31" s="116"/>
       <c r="B31" s="1">
         <v>30</v>
       </c>
@@ -2816,12 +2936,12 @@
       <c r="E31" s="13">
         <v>1</v>
       </c>
-      <c r="F31" s="95"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="105"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="107"/>
     </row>
     <row r="32" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A32" s="107"/>
+      <c r="A32" s="116"/>
       <c r="B32" s="1">
         <v>31</v>
       </c>
@@ -2834,12 +2954,12 @@
       <c r="E32" s="13">
         <v>1</v>
       </c>
-      <c r="F32" s="95"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="105"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="102"/>
+      <c r="H32" s="107"/>
     </row>
     <row r="33" spans="1:9" ht="18">
-      <c r="A33" s="107"/>
+      <c r="A33" s="116"/>
       <c r="B33" s="1">
         <v>32</v>
       </c>
@@ -2852,18 +2972,18 @@
       <c r="E33" s="13">
         <v>1</v>
       </c>
-      <c r="F33" s="95" t="s">
-        <v>212</v>
-      </c>
-      <c r="G33" s="95">
+      <c r="F33" s="102" t="s">
+        <v>211</v>
+      </c>
+      <c r="G33" s="102">
         <v>4</v>
       </c>
-      <c r="H33" s="105" t="s">
-        <v>252</v>
+      <c r="H33" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="18">
-      <c r="A34" s="107"/>
+      <c r="A34" s="116"/>
       <c r="B34" s="1">
         <v>33</v>
       </c>
@@ -2876,12 +2996,12 @@
       <c r="E34" s="13">
         <v>1</v>
       </c>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="105"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="107"/>
     </row>
     <row r="35" spans="1:9" ht="18">
-      <c r="A35" s="107"/>
+      <c r="A35" s="116"/>
       <c r="B35" s="1">
         <v>34</v>
       </c>
@@ -2894,12 +3014,12 @@
       <c r="E35" s="13">
         <v>1</v>
       </c>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="105"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="107"/>
     </row>
     <row r="36" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A36" s="107"/>
+      <c r="A36" s="116"/>
       <c r="B36" s="1">
         <v>35</v>
       </c>
@@ -2912,12 +3032,12 @@
       <c r="E36" s="13">
         <v>1</v>
       </c>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="105"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="102"/>
+      <c r="H36" s="107"/>
     </row>
     <row r="37" spans="1:9" ht="18">
-      <c r="A37" s="107"/>
+      <c r="A37" s="116"/>
       <c r="B37" s="1">
         <v>36</v>
       </c>
@@ -2930,18 +3050,18 @@
       <c r="E37" s="13">
         <v>1</v>
       </c>
-      <c r="F37" s="95" t="s">
-        <v>213</v>
-      </c>
-      <c r="G37" s="95">
+      <c r="F37" s="102" t="s">
+        <v>212</v>
+      </c>
+      <c r="G37" s="102">
         <v>4</v>
       </c>
-      <c r="H37" s="105" t="s">
-        <v>252</v>
+      <c r="H37" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="18">
-      <c r="A38" s="107"/>
+      <c r="A38" s="116"/>
       <c r="B38" s="1">
         <v>37</v>
       </c>
@@ -2954,12 +3074,12 @@
       <c r="E38" s="13">
         <v>1</v>
       </c>
-      <c r="F38" s="95"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="105"/>
+      <c r="F38" s="102"/>
+      <c r="G38" s="102"/>
+      <c r="H38" s="107"/>
     </row>
     <row r="39" spans="1:9" ht="18">
-      <c r="A39" s="107"/>
+      <c r="A39" s="116"/>
       <c r="B39" s="1">
         <v>38</v>
       </c>
@@ -2972,12 +3092,12 @@
       <c r="E39" s="13">
         <v>1</v>
       </c>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="105"/>
+      <c r="F39" s="102"/>
+      <c r="G39" s="102"/>
+      <c r="H39" s="107"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A40" s="107"/>
+      <c r="A40" s="116"/>
       <c r="B40" s="1">
         <v>39</v>
       </c>
@@ -2990,12 +3110,12 @@
       <c r="E40" s="13">
         <v>1</v>
       </c>
-      <c r="F40" s="95"/>
-      <c r="G40" s="95"/>
-      <c r="H40" s="105"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="102"/>
+      <c r="H40" s="107"/>
     </row>
     <row r="41" spans="1:9" ht="18">
-      <c r="A41" s="107"/>
+      <c r="A41" s="116"/>
       <c r="B41" s="1">
         <v>40</v>
       </c>
@@ -3008,18 +3128,18 @@
       <c r="E41" s="13">
         <v>2</v>
       </c>
-      <c r="F41" s="95" t="s">
-        <v>214</v>
-      </c>
-      <c r="G41" s="95">
+      <c r="F41" s="102" t="s">
+        <v>213</v>
+      </c>
+      <c r="G41" s="102">
         <v>4</v>
       </c>
-      <c r="H41" s="105" t="s">
-        <v>252</v>
+      <c r="H41" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A42" s="107"/>
+      <c r="A42" s="116"/>
       <c r="B42" s="1">
         <v>41</v>
       </c>
@@ -3032,12 +3152,12 @@
       <c r="E42" s="13">
         <v>2</v>
       </c>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="105"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="107"/>
     </row>
     <row r="43" spans="1:9" ht="18">
-      <c r="A43" s="107"/>
+      <c r="A43" s="116"/>
       <c r="B43" s="1">
         <v>42</v>
       </c>
@@ -3050,19 +3170,19 @@
       <c r="E43" s="13">
         <v>1</v>
       </c>
-      <c r="F43" s="95" t="s">
-        <v>215</v>
-      </c>
-      <c r="G43" s="95">
+      <c r="F43" s="102" t="s">
+        <v>214</v>
+      </c>
+      <c r="G43" s="102">
         <v>4</v>
       </c>
-      <c r="H43" s="105" t="s">
-        <v>252</v>
+      <c r="H43" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" ht="18">
-      <c r="A44" s="107"/>
+      <c r="A44" s="116"/>
       <c r="B44" s="1">
         <v>43</v>
       </c>
@@ -3075,47 +3195,47 @@
       <c r="E44" s="13">
         <v>1</v>
       </c>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="105"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="102"/>
+      <c r="H44" s="107"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" ht="18">
-      <c r="A45" s="107"/>
+      <c r="A45" s="116"/>
       <c r="B45" s="1">
         <v>44</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E45" s="13">
         <v>1</v>
       </c>
-      <c r="F45" s="95"/>
-      <c r="G45" s="95"/>
-      <c r="H45" s="105"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="102"/>
+      <c r="H45" s="107"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" ht="18.75" thickBot="1">
-      <c r="A46" s="108"/>
+      <c r="A46" s="118"/>
       <c r="B46" s="1">
         <v>45</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E46" s="13">
         <v>1</v>
       </c>
-      <c r="F46" s="95"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="105"/>
+      <c r="F46" s="102"/>
+      <c r="G46" s="102"/>
+      <c r="H46" s="107"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" ht="18">
-      <c r="A47" s="109" t="s">
+      <c r="A47" s="112" t="s">
         <v>141</v>
       </c>
       <c r="B47" s="1">
@@ -3130,19 +3250,19 @@
       <c r="E47" s="13">
         <v>1</v>
       </c>
-      <c r="F47" s="95" t="s">
-        <v>216</v>
-      </c>
-      <c r="G47" s="95">
+      <c r="F47" s="102" t="s">
+        <v>215</v>
+      </c>
+      <c r="G47" s="102">
         <v>4</v>
       </c>
-      <c r="H47" s="105" t="s">
-        <v>252</v>
+      <c r="H47" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" ht="18">
-      <c r="A48" s="110"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="1">
         <v>47</v>
       </c>
@@ -3155,12 +3275,12 @@
       <c r="E48" s="13">
         <v>1</v>
       </c>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="105"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="102"/>
+      <c r="H48" s="107"/>
     </row>
     <row r="49" spans="1:8" ht="18">
-      <c r="A49" s="110"/>
+      <c r="A49" s="113"/>
       <c r="B49" s="1">
         <v>48</v>
       </c>
@@ -3173,12 +3293,12 @@
       <c r="E49" s="13">
         <v>1</v>
       </c>
-      <c r="F49" s="95"/>
-      <c r="G49" s="95"/>
-      <c r="H49" s="105"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="102"/>
+      <c r="H49" s="107"/>
     </row>
     <row r="50" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A50" s="110"/>
+      <c r="A50" s="113"/>
       <c r="B50" s="1">
         <v>49</v>
       </c>
@@ -3189,12 +3309,12 @@
       <c r="E50" s="13">
         <v>1</v>
       </c>
-      <c r="F50" s="95"/>
-      <c r="G50" s="95"/>
-      <c r="H50" s="105"/>
+      <c r="F50" s="102"/>
+      <c r="G50" s="102"/>
+      <c r="H50" s="107"/>
     </row>
     <row r="51" spans="1:8" ht="18">
-      <c r="A51" s="110"/>
+      <c r="A51" s="113"/>
       <c r="B51" s="1">
         <v>50</v>
       </c>
@@ -3205,18 +3325,18 @@
       <c r="E51" s="66">
         <v>1</v>
       </c>
-      <c r="F51" s="100" t="s">
-        <v>217</v>
-      </c>
-      <c r="G51" s="100">
+      <c r="F51" s="108" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" s="108">
         <v>3</v>
       </c>
-      <c r="H51" s="105" t="s">
-        <v>252</v>
+      <c r="H51" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="18">
-      <c r="A52" s="110"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="1">
         <v>51</v>
       </c>
@@ -3224,17 +3344,17 @@
         <v>4</v>
       </c>
       <c r="D52" s="37" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E52" s="66">
         <v>1</v>
       </c>
-      <c r="F52" s="100"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="105"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="107"/>
     </row>
     <row r="53" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A53" s="110"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="1">
         <v>52</v>
       </c>
@@ -3242,17 +3362,17 @@
         <v>5</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E53" s="66">
         <v>1</v>
       </c>
-      <c r="F53" s="100"/>
-      <c r="G53" s="100"/>
-      <c r="H53" s="105"/>
+      <c r="F53" s="108"/>
+      <c r="G53" s="108"/>
+      <c r="H53" s="107"/>
     </row>
     <row r="54" spans="1:8" ht="18">
-      <c r="A54" s="110"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="1">
         <v>53</v>
       </c>
@@ -3263,18 +3383,18 @@
       <c r="E54" s="13">
         <v>2</v>
       </c>
-      <c r="F54" s="95" t="s">
-        <v>218</v>
-      </c>
-      <c r="G54" s="95">
+      <c r="F54" s="102" t="s">
+        <v>217</v>
+      </c>
+      <c r="G54" s="102">
         <v>5</v>
       </c>
-      <c r="H54" s="105" t="s">
-        <v>252</v>
+      <c r="H54" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="18">
-      <c r="A55" s="110"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="1">
         <v>54</v>
       </c>
@@ -3285,12 +3405,12 @@
       <c r="E55" s="13">
         <v>1</v>
       </c>
-      <c r="F55" s="95"/>
-      <c r="G55" s="95"/>
-      <c r="H55" s="105"/>
+      <c r="F55" s="102"/>
+      <c r="G55" s="102"/>
+      <c r="H55" s="107"/>
     </row>
     <row r="56" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A56" s="110"/>
+      <c r="A56" s="113"/>
       <c r="B56" s="1">
         <v>55</v>
       </c>
@@ -3303,12 +3423,12 @@
       <c r="E56" s="13">
         <v>2</v>
       </c>
-      <c r="F56" s="95"/>
-      <c r="G56" s="95"/>
-      <c r="H56" s="105"/>
+      <c r="F56" s="102"/>
+      <c r="G56" s="102"/>
+      <c r="H56" s="107"/>
     </row>
     <row r="57" spans="1:8" ht="18">
-      <c r="A57" s="110"/>
+      <c r="A57" s="113"/>
       <c r="B57" s="1">
         <v>56</v>
       </c>
@@ -3321,18 +3441,18 @@
       <c r="E57" s="13">
         <v>2</v>
       </c>
-      <c r="F57" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="G57" s="95">
+      <c r="F57" s="102" t="s">
+        <v>218</v>
+      </c>
+      <c r="G57" s="102">
         <v>3</v>
       </c>
-      <c r="H57" s="105" t="s">
-        <v>252</v>
+      <c r="H57" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A58" s="110"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="1">
         <v>57</v>
       </c>
@@ -3345,12 +3465,12 @@
       <c r="E58" s="13">
         <v>1</v>
       </c>
-      <c r="F58" s="95"/>
-      <c r="G58" s="95"/>
-      <c r="H58" s="105"/>
+      <c r="F58" s="102"/>
+      <c r="G58" s="102"/>
+      <c r="H58" s="107"/>
     </row>
     <row r="59" spans="1:8" ht="18">
-      <c r="A59" s="110"/>
+      <c r="A59" s="113"/>
       <c r="B59" s="1">
         <v>58</v>
       </c>
@@ -3363,18 +3483,18 @@
       <c r="E59" s="13">
         <v>1</v>
       </c>
-      <c r="F59" s="95" t="s">
-        <v>220</v>
-      </c>
-      <c r="G59" s="95">
+      <c r="F59" s="102" t="s">
+        <v>219</v>
+      </c>
+      <c r="G59" s="102">
         <v>4</v>
       </c>
-      <c r="H59" s="105" t="s">
-        <v>252</v>
+      <c r="H59" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="18">
-      <c r="A60" s="110"/>
+      <c r="A60" s="113"/>
       <c r="B60" s="1">
         <v>59</v>
       </c>
@@ -3387,12 +3507,12 @@
       <c r="E60" s="13">
         <v>1</v>
       </c>
-      <c r="F60" s="95"/>
-      <c r="G60" s="95"/>
-      <c r="H60" s="105"/>
+      <c r="F60" s="102"/>
+      <c r="G60" s="102"/>
+      <c r="H60" s="107"/>
     </row>
     <row r="61" spans="1:8" ht="18">
-      <c r="A61" s="110"/>
+      <c r="A61" s="113"/>
       <c r="B61" s="1">
         <v>60</v>
       </c>
@@ -3405,12 +3525,12 @@
       <c r="E61" s="13">
         <v>1</v>
       </c>
-      <c r="F61" s="95"/>
-      <c r="G61" s="95"/>
-      <c r="H61" s="105"/>
+      <c r="F61" s="102"/>
+      <c r="G61" s="102"/>
+      <c r="H61" s="107"/>
     </row>
     <row r="62" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A62" s="110"/>
+      <c r="A62" s="113"/>
       <c r="B62" s="1">
         <v>61</v>
       </c>
@@ -3423,34 +3543,34 @@
       <c r="E62" s="52">
         <v>1</v>
       </c>
-      <c r="F62" s="95"/>
-      <c r="G62" s="95"/>
-      <c r="H62" s="105"/>
+      <c r="F62" s="102"/>
+      <c r="G62" s="102"/>
+      <c r="H62" s="107"/>
     </row>
     <row r="63" spans="1:8" ht="18">
-      <c r="A63" s="110"/>
+      <c r="A63" s="113"/>
       <c r="B63" s="1">
         <v>62</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E63" s="80">
         <v>1</v>
       </c>
-      <c r="F63" s="101" t="s">
-        <v>221</v>
-      </c>
-      <c r="G63" s="95">
+      <c r="F63" s="109" t="s">
+        <v>220</v>
+      </c>
+      <c r="G63" s="102">
         <v>4</v>
       </c>
-      <c r="H63" s="105" t="s">
-        <v>252</v>
+      <c r="H63" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A64" s="110"/>
+      <c r="A64" s="113"/>
       <c r="B64" s="1">
         <v>63</v>
       </c>
@@ -3463,12 +3583,12 @@
       <c r="E64" s="81">
         <v>1</v>
       </c>
-      <c r="F64" s="102"/>
-      <c r="G64" s="95"/>
-      <c r="H64" s="105"/>
+      <c r="F64" s="110"/>
+      <c r="G64" s="102"/>
+      <c r="H64" s="107"/>
     </row>
     <row r="65" spans="1:10" ht="18">
-      <c r="A65" s="110"/>
+      <c r="A65" s="113"/>
       <c r="B65" s="1">
         <v>64</v>
       </c>
@@ -3481,12 +3601,12 @@
       <c r="E65" s="80">
         <v>1</v>
       </c>
-      <c r="F65" s="102"/>
-      <c r="G65" s="95"/>
-      <c r="H65" s="105"/>
+      <c r="F65" s="110"/>
+      <c r="G65" s="102"/>
+      <c r="H65" s="107"/>
     </row>
     <row r="66" spans="1:10" ht="18.75" thickBot="1">
-      <c r="A66" s="110"/>
+      <c r="A66" s="113"/>
       <c r="B66" s="1">
         <v>65</v>
       </c>
@@ -3499,12 +3619,12 @@
       <c r="E66" s="81">
         <v>1</v>
       </c>
-      <c r="F66" s="103"/>
-      <c r="G66" s="95"/>
-      <c r="H66" s="105"/>
+      <c r="F66" s="111"/>
+      <c r="G66" s="102"/>
+      <c r="H66" s="107"/>
     </row>
     <row r="67" spans="1:10" ht="18">
-      <c r="A67" s="110"/>
+      <c r="A67" s="113"/>
       <c r="B67" s="1">
         <v>66</v>
       </c>
@@ -3517,56 +3637,56 @@
       <c r="E67" s="68">
         <v>1</v>
       </c>
-      <c r="F67" s="95" t="s">
-        <v>222</v>
-      </c>
-      <c r="G67" s="95">
+      <c r="F67" s="102" t="s">
+        <v>221</v>
+      </c>
+      <c r="G67" s="102">
         <v>4</v>
       </c>
-      <c r="H67" s="105" t="s">
-        <v>252</v>
+      <c r="H67" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
     <row r="68" spans="1:10" ht="18">
-      <c r="A68" s="110"/>
+      <c r="A68" s="113"/>
       <c r="B68" s="1">
         <v>67</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E68" s="13">
         <v>1</v>
       </c>
-      <c r="F68" s="95"/>
-      <c r="G68" s="95"/>
-      <c r="H68" s="105"/>
+      <c r="F68" s="102"/>
+      <c r="G68" s="102"/>
+      <c r="H68" s="107"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
     <row r="69" spans="1:10" ht="18">
-      <c r="A69" s="110"/>
+      <c r="A69" s="113"/>
       <c r="B69" s="1">
         <v>68</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E69" s="13">
         <v>1</v>
       </c>
-      <c r="F69" s="95"/>
-      <c r="G69" s="95"/>
-      <c r="H69" s="105"/>
+      <c r="F69" s="102"/>
+      <c r="G69" s="102"/>
+      <c r="H69" s="107"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
     <row r="70" spans="1:10" ht="18.75" thickBot="1">
-      <c r="A70" s="110"/>
+      <c r="A70" s="113"/>
       <c r="B70" s="1">
         <v>69</v>
       </c>
@@ -3579,14 +3699,14 @@
       <c r="E70" s="13">
         <v>1</v>
       </c>
-      <c r="F70" s="95"/>
-      <c r="G70" s="95"/>
-      <c r="H70" s="105"/>
+      <c r="F70" s="102"/>
+      <c r="G70" s="102"/>
+      <c r="H70" s="107"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="1:10" ht="18">
-      <c r="A71" s="110"/>
+      <c r="A71" s="113"/>
       <c r="B71" s="1">
         <v>70</v>
       </c>
@@ -3599,20 +3719,20 @@
       <c r="E71" s="13">
         <v>1</v>
       </c>
-      <c r="F71" s="95" t="s">
-        <v>223</v>
-      </c>
-      <c r="G71" s="95">
+      <c r="F71" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="G71" s="102">
         <v>4</v>
       </c>
-      <c r="H71" s="105" t="s">
-        <v>252</v>
+      <c r="H71" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="1:10" ht="18">
-      <c r="A72" s="110"/>
+      <c r="A72" s="113"/>
       <c r="B72" s="1">
         <v>71</v>
       </c>
@@ -3625,14 +3745,14 @@
       <c r="E72" s="13">
         <v>1</v>
       </c>
-      <c r="F72" s="95"/>
-      <c r="G72" s="95"/>
-      <c r="H72" s="105"/>
+      <c r="F72" s="102"/>
+      <c r="G72" s="102"/>
+      <c r="H72" s="107"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="1:10" ht="18">
-      <c r="A73" s="110"/>
+      <c r="A73" s="113"/>
       <c r="B73" s="1">
         <v>72</v>
       </c>
@@ -3643,14 +3763,14 @@
       <c r="E73" s="13">
         <v>1</v>
       </c>
-      <c r="F73" s="95"/>
-      <c r="G73" s="95"/>
-      <c r="H73" s="105"/>
+      <c r="F73" s="102"/>
+      <c r="G73" s="102"/>
+      <c r="H73" s="107"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
     <row r="74" spans="1:10" ht="18.75" thickBot="1">
-      <c r="A74" s="112"/>
+      <c r="A74" s="117"/>
       <c r="B74" s="1">
         <v>73</v>
       </c>
@@ -3663,14 +3783,14 @@
       <c r="E74" s="13">
         <v>1</v>
       </c>
-      <c r="F74" s="95"/>
-      <c r="G74" s="95"/>
-      <c r="H74" s="105"/>
+      <c r="F74" s="102"/>
+      <c r="G74" s="102"/>
+      <c r="H74" s="107"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
     <row r="75" spans="1:10" ht="18">
-      <c r="A75" s="109" t="s">
+      <c r="A75" s="112" t="s">
         <v>142</v>
       </c>
       <c r="B75" s="1">
@@ -3685,20 +3805,20 @@
       <c r="E75" s="13">
         <v>1</v>
       </c>
-      <c r="F75" s="95" t="s">
-        <v>224</v>
-      </c>
-      <c r="G75" s="95">
+      <c r="F75" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="G75" s="102">
         <v>4</v>
       </c>
-      <c r="H75" s="105" t="s">
-        <v>252</v>
+      <c r="H75" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
     <row r="76" spans="1:10" ht="18">
-      <c r="A76" s="110"/>
+      <c r="A76" s="113"/>
       <c r="B76" s="1">
         <v>75</v>
       </c>
@@ -3709,12 +3829,12 @@
       <c r="E76" s="13">
         <v>1</v>
       </c>
-      <c r="F76" s="95"/>
-      <c r="G76" s="95"/>
-      <c r="H76" s="105"/>
+      <c r="F76" s="102"/>
+      <c r="G76" s="102"/>
+      <c r="H76" s="107"/>
     </row>
     <row r="77" spans="1:10" ht="18">
-      <c r="A77" s="110"/>
+      <c r="A77" s="113"/>
       <c r="B77" s="1">
         <v>76</v>
       </c>
@@ -3727,28 +3847,28 @@
       <c r="E77" s="13">
         <v>1</v>
       </c>
-      <c r="F77" s="95"/>
-      <c r="G77" s="95"/>
-      <c r="H77" s="105"/>
+      <c r="F77" s="102"/>
+      <c r="G77" s="102"/>
+      <c r="H77" s="107"/>
     </row>
     <row r="78" spans="1:10" ht="18.75" thickBot="1">
-      <c r="A78" s="110"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="1">
         <v>77</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E78" s="13">
         <v>1</v>
       </c>
-      <c r="F78" s="95"/>
-      <c r="G78" s="95"/>
-      <c r="H78" s="105"/>
+      <c r="F78" s="102"/>
+      <c r="G78" s="102"/>
+      <c r="H78" s="107"/>
     </row>
     <row r="79" spans="1:10" ht="18">
-      <c r="A79" s="110"/>
+      <c r="A79" s="113"/>
       <c r="B79" s="1">
         <v>78</v>
       </c>
@@ -3761,18 +3881,18 @@
       <c r="E79" s="13">
         <v>2</v>
       </c>
-      <c r="F79" s="95" t="s">
-        <v>225</v>
-      </c>
-      <c r="G79" s="95">
+      <c r="F79" s="102" t="s">
+        <v>224</v>
+      </c>
+      <c r="G79" s="102">
         <v>4</v>
       </c>
-      <c r="H79" s="105" t="s">
-        <v>252</v>
+      <c r="H79" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="18">
-      <c r="A80" s="110"/>
+      <c r="A80" s="113"/>
       <c r="B80" s="1">
         <v>79</v>
       </c>
@@ -3785,12 +3905,12 @@
       <c r="E80" s="13">
         <v>1</v>
       </c>
-      <c r="F80" s="95"/>
-      <c r="G80" s="95"/>
-      <c r="H80" s="105"/>
+      <c r="F80" s="102"/>
+      <c r="G80" s="102"/>
+      <c r="H80" s="107"/>
     </row>
     <row r="81" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A81" s="110"/>
+      <c r="A81" s="113"/>
       <c r="B81" s="1">
         <v>80</v>
       </c>
@@ -3803,12 +3923,12 @@
       <c r="E81" s="13">
         <v>1</v>
       </c>
-      <c r="F81" s="95"/>
-      <c r="G81" s="95"/>
-      <c r="H81" s="105"/>
+      <c r="F81" s="102"/>
+      <c r="G81" s="102"/>
+      <c r="H81" s="107"/>
     </row>
     <row r="82" spans="1:15" ht="18">
-      <c r="A82" s="110"/>
+      <c r="A82" s="113"/>
       <c r="B82" s="1">
         <v>81</v>
       </c>
@@ -3821,18 +3941,18 @@
       <c r="E82" s="13">
         <v>2</v>
       </c>
-      <c r="F82" s="95" t="s">
-        <v>226</v>
-      </c>
-      <c r="G82" s="95">
+      <c r="F82" s="102" t="s">
+        <v>225</v>
+      </c>
+      <c r="G82" s="102">
         <v>4</v>
       </c>
-      <c r="H82" s="105" t="s">
-        <v>252</v>
+      <c r="H82" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A83" s="110"/>
+      <c r="A83" s="113"/>
       <c r="B83" s="1">
         <v>82</v>
       </c>
@@ -3845,12 +3965,12 @@
       <c r="E83" s="13">
         <v>2</v>
       </c>
-      <c r="F83" s="95"/>
-      <c r="G83" s="95"/>
-      <c r="H83" s="105"/>
+      <c r="F83" s="102"/>
+      <c r="G83" s="102"/>
+      <c r="H83" s="107"/>
     </row>
     <row r="84" spans="1:15" ht="18">
-      <c r="A84" s="110"/>
+      <c r="A84" s="113"/>
       <c r="B84" s="1">
         <v>83</v>
       </c>
@@ -3858,39 +3978,39 @@
         <v>8</v>
       </c>
       <c r="D84" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E84" s="13">
         <v>1</v>
       </c>
-      <c r="F84" s="95" t="s">
-        <v>227</v>
-      </c>
-      <c r="G84" s="95">
+      <c r="F84" s="102" t="s">
+        <v>226</v>
+      </c>
+      <c r="G84" s="102">
         <v>4</v>
       </c>
-      <c r="H84" s="105" t="s">
-        <v>252</v>
+      <c r="H84" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="18">
-      <c r="A85" s="110"/>
+      <c r="A85" s="113"/>
       <c r="B85" s="1">
         <v>84</v>
       </c>
       <c r="C85" s="16"/>
       <c r="D85" s="40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E85" s="13">
         <v>2</v>
       </c>
-      <c r="F85" s="95"/>
-      <c r="G85" s="95"/>
-      <c r="H85" s="105"/>
+      <c r="F85" s="102"/>
+      <c r="G85" s="102"/>
+      <c r="H85" s="107"/>
     </row>
     <row r="86" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A86" s="110"/>
+      <c r="A86" s="113"/>
       <c r="B86" s="1">
         <v>85</v>
       </c>
@@ -3903,12 +4023,12 @@
       <c r="E86" s="13">
         <v>1</v>
       </c>
-      <c r="F86" s="95"/>
-      <c r="G86" s="95"/>
-      <c r="H86" s="105"/>
+      <c r="F86" s="102"/>
+      <c r="G86" s="102"/>
+      <c r="H86" s="107"/>
     </row>
     <row r="87" spans="1:15" ht="18">
-      <c r="A87" s="110"/>
+      <c r="A87" s="113"/>
       <c r="B87" s="1">
         <v>86</v>
       </c>
@@ -3921,18 +4041,18 @@
       <c r="E87" s="13">
         <v>1</v>
       </c>
-      <c r="F87" s="95" t="s">
-        <v>228</v>
-      </c>
-      <c r="G87" s="95">
+      <c r="F87" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="G87" s="102">
         <v>4</v>
       </c>
-      <c r="H87" s="105" t="s">
-        <v>252</v>
+      <c r="H87" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="18">
-      <c r="A88" s="110"/>
+      <c r="A88" s="113"/>
       <c r="B88" s="1">
         <v>87</v>
       </c>
@@ -3945,12 +4065,12 @@
       <c r="E88" s="13">
         <v>1</v>
       </c>
-      <c r="F88" s="95"/>
-      <c r="G88" s="95"/>
-      <c r="H88" s="105"/>
+      <c r="F88" s="102"/>
+      <c r="G88" s="102"/>
+      <c r="H88" s="107"/>
     </row>
     <row r="89" spans="1:15" ht="18">
-      <c r="A89" s="110"/>
+      <c r="A89" s="113"/>
       <c r="B89" s="1">
         <v>88</v>
       </c>
@@ -3963,12 +4083,12 @@
       <c r="E89" s="13">
         <v>1</v>
       </c>
-      <c r="F89" s="95"/>
-      <c r="G89" s="95"/>
-      <c r="H89" s="105"/>
+      <c r="F89" s="102"/>
+      <c r="G89" s="102"/>
+      <c r="H89" s="107"/>
     </row>
     <row r="90" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A90" s="110"/>
+      <c r="A90" s="113"/>
       <c r="B90" s="1">
         <v>89</v>
       </c>
@@ -3981,12 +4101,12 @@
       <c r="E90" s="13">
         <v>1</v>
       </c>
-      <c r="F90" s="95"/>
-      <c r="G90" s="95"/>
-      <c r="H90" s="105"/>
+      <c r="F90" s="102"/>
+      <c r="G90" s="102"/>
+      <c r="H90" s="107"/>
     </row>
     <row r="91" spans="1:15" ht="18">
-      <c r="A91" s="110"/>
+      <c r="A91" s="113"/>
       <c r="B91" s="1">
         <v>90</v>
       </c>
@@ -3999,24 +4119,24 @@
       <c r="E91" s="13">
         <v>2</v>
       </c>
-      <c r="F91" s="104" t="s">
-        <v>229</v>
-      </c>
-      <c r="G91" s="96">
+      <c r="F91" s="119" t="s">
+        <v>228</v>
+      </c>
+      <c r="G91" s="103">
         <v>6</v>
       </c>
-      <c r="H91" s="127" t="s">
-        <v>257</v>
+      <c r="H91" s="132" t="s">
+        <v>256</v>
       </c>
       <c r="J91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K91" s="72" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="18">
-      <c r="A92" s="110"/>
+      <c r="A92" s="113"/>
       <c r="B92" s="1">
         <v>91</v>
       </c>
@@ -4024,23 +4144,23 @@
         <v>15</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E92" s="13">
         <v>1</v>
       </c>
-      <c r="F92" s="104"/>
-      <c r="G92" s="96"/>
-      <c r="H92" s="127"/>
+      <c r="F92" s="119"/>
+      <c r="G92" s="103"/>
+      <c r="H92" s="132"/>
       <c r="J92" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A93" s="110"/>
+      <c r="A93" s="113"/>
       <c r="B93" s="1">
         <v>92</v>
       </c>
@@ -4053,18 +4173,18 @@
       <c r="E93" s="13">
         <v>1</v>
       </c>
-      <c r="F93" s="104"/>
-      <c r="G93" s="96"/>
-      <c r="H93" s="127"/>
+      <c r="F93" s="119"/>
+      <c r="G93" s="103"/>
+      <c r="H93" s="132"/>
       <c r="J93" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K93" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="18">
-      <c r="A94" s="110"/>
+      <c r="A94" s="113"/>
       <c r="B94" s="1">
         <v>93</v>
       </c>
@@ -4077,17 +4197,17 @@
       <c r="E94" s="13">
         <v>1</v>
       </c>
-      <c r="F94" s="95" t="s">
-        <v>236</v>
-      </c>
-      <c r="G94" s="97"/>
-      <c r="H94" s="128"/>
+      <c r="F94" s="102" t="s">
+        <v>235</v>
+      </c>
+      <c r="G94" s="104"/>
+      <c r="H94" s="133"/>
       <c r="I94" s="5"/>
       <c r="J94" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L94" s="5"/>
       <c r="M94" s="5"/>
@@ -4095,7 +4215,7 @@
       <c r="O94" s="5"/>
     </row>
     <row r="95" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A95" s="112"/>
+      <c r="A95" s="117"/>
       <c r="B95" s="1">
         <v>94</v>
       </c>
@@ -4106,15 +4226,15 @@
       <c r="E95" s="13">
         <v>1</v>
       </c>
-      <c r="F95" s="95"/>
-      <c r="G95" s="97"/>
-      <c r="H95" s="128"/>
+      <c r="F95" s="102"/>
+      <c r="G95" s="104"/>
+      <c r="H95" s="133"/>
       <c r="I95" s="5"/>
       <c r="J95" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K95" s="57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L95" s="5"/>
       <c r="M95" s="5"/>
@@ -4122,7 +4242,7 @@
       <c r="O95" s="5"/>
     </row>
     <row r="96" spans="1:15" ht="18">
-      <c r="A96" s="109" t="s">
+      <c r="A96" s="112" t="s">
         <v>143</v>
       </c>
       <c r="B96" s="1">
@@ -4137,21 +4257,21 @@
       <c r="E96" s="13">
         <v>1</v>
       </c>
-      <c r="F96" s="95" t="s">
-        <v>230</v>
-      </c>
-      <c r="G96" s="95">
+      <c r="F96" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="G96" s="102">
         <v>4</v>
       </c>
-      <c r="H96" s="105" t="s">
-        <v>252</v>
+      <c r="H96" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I96" s="5"/>
       <c r="J96" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K96" s="57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L96" s="5"/>
       <c r="M96" s="5"/>
@@ -4159,7 +4279,7 @@
       <c r="O96" s="5"/>
     </row>
     <row r="97" spans="1:15" ht="18">
-      <c r="A97" s="110"/>
+      <c r="A97" s="113"/>
       <c r="B97" s="1">
         <v>96</v>
       </c>
@@ -4172,9 +4292,9 @@
       <c r="E97" s="13">
         <v>1</v>
       </c>
-      <c r="F97" s="95"/>
-      <c r="G97" s="95"/>
-      <c r="H97" s="105"/>
+      <c r="F97" s="102"/>
+      <c r="G97" s="102"/>
+      <c r="H97" s="107"/>
       <c r="I97" s="5"/>
       <c r="J97" s="4"/>
       <c r="K97" s="57"/>
@@ -4184,7 +4304,7 @@
       <c r="O97" s="5"/>
     </row>
     <row r="98" spans="1:15" ht="18">
-      <c r="A98" s="110"/>
+      <c r="A98" s="113"/>
       <c r="B98" s="1">
         <v>97</v>
       </c>
@@ -4197,9 +4317,9 @@
       <c r="E98" s="13">
         <v>1</v>
       </c>
-      <c r="F98" s="95"/>
-      <c r="G98" s="95"/>
-      <c r="H98" s="105"/>
+      <c r="F98" s="102"/>
+      <c r="G98" s="102"/>
+      <c r="H98" s="107"/>
       <c r="I98" s="5"/>
       <c r="J98" s="4"/>
       <c r="K98" s="57"/>
@@ -4209,7 +4329,7 @@
       <c r="O98" s="5"/>
     </row>
     <row r="99" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A99" s="110"/>
+      <c r="A99" s="113"/>
       <c r="B99" s="1">
         <v>98</v>
       </c>
@@ -4222,9 +4342,9 @@
       <c r="E99" s="13">
         <v>1</v>
       </c>
-      <c r="F99" s="95"/>
-      <c r="G99" s="95"/>
-      <c r="H99" s="105"/>
+      <c r="F99" s="102"/>
+      <c r="G99" s="102"/>
+      <c r="H99" s="107"/>
       <c r="I99" s="5"/>
       <c r="J99" s="4"/>
       <c r="K99" s="57"/>
@@ -4234,7 +4354,7 @@
       <c r="O99" s="5"/>
     </row>
     <row r="100" spans="1:15" ht="18">
-      <c r="A100" s="110"/>
+      <c r="A100" s="113"/>
       <c r="B100" s="1">
         <v>99</v>
       </c>
@@ -4247,14 +4367,14 @@
       <c r="E100" s="13">
         <v>1</v>
       </c>
-      <c r="F100" s="95" t="s">
-        <v>231</v>
-      </c>
-      <c r="G100" s="95">
+      <c r="F100" s="102" t="s">
+        <v>230</v>
+      </c>
+      <c r="G100" s="102">
         <v>4</v>
       </c>
-      <c r="H100" s="105" t="s">
-        <v>252</v>
+      <c r="H100" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I100" s="5"/>
       <c r="J100" s="4"/>
@@ -4265,7 +4385,7 @@
       <c r="O100" s="5"/>
     </row>
     <row r="101" spans="1:15" ht="18">
-      <c r="A101" s="110"/>
+      <c r="A101" s="113"/>
       <c r="B101" s="1">
         <v>100</v>
       </c>
@@ -4278,9 +4398,9 @@
       <c r="E101" s="13">
         <v>1</v>
       </c>
-      <c r="F101" s="95"/>
-      <c r="G101" s="95"/>
-      <c r="H101" s="105"/>
+      <c r="F101" s="102"/>
+      <c r="G101" s="102"/>
+      <c r="H101" s="107"/>
       <c r="I101" s="5"/>
       <c r="J101" s="4"/>
       <c r="K101" s="57"/>
@@ -4290,7 +4410,7 @@
       <c r="O101" s="5"/>
     </row>
     <row r="102" spans="1:15" ht="18">
-      <c r="A102" s="110"/>
+      <c r="A102" s="113"/>
       <c r="B102" s="1">
         <v>101</v>
       </c>
@@ -4303,9 +4423,9 @@
       <c r="E102" s="13">
         <v>1</v>
       </c>
-      <c r="F102" s="95"/>
-      <c r="G102" s="95"/>
-      <c r="H102" s="105"/>
+      <c r="F102" s="102"/>
+      <c r="G102" s="102"/>
+      <c r="H102" s="107"/>
       <c r="I102" s="4"/>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
@@ -4315,7 +4435,7 @@
       <c r="O102" s="5"/>
     </row>
     <row r="103" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A103" s="110"/>
+      <c r="A103" s="113"/>
       <c r="B103" s="1">
         <v>102</v>
       </c>
@@ -4328,9 +4448,9 @@
       <c r="E103" s="13">
         <v>1</v>
       </c>
-      <c r="F103" s="95"/>
-      <c r="G103" s="95"/>
-      <c r="H103" s="105"/>
+      <c r="F103" s="102"/>
+      <c r="G103" s="102"/>
+      <c r="H103" s="107"/>
       <c r="I103" s="4"/>
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
@@ -4340,7 +4460,7 @@
       <c r="O103" s="5"/>
     </row>
     <row r="104" spans="1:15" ht="18">
-      <c r="A104" s="110"/>
+      <c r="A104" s="113"/>
       <c r="B104" s="1">
         <v>103</v>
       </c>
@@ -4353,14 +4473,14 @@
       <c r="E104" s="13">
         <v>1</v>
       </c>
-      <c r="F104" s="95" t="s">
-        <v>232</v>
-      </c>
-      <c r="G104" s="95">
+      <c r="F104" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="G104" s="102">
         <v>5</v>
       </c>
-      <c r="H104" s="105" t="s">
-        <v>252</v>
+      <c r="H104" s="107" t="s">
+        <v>251</v>
       </c>
       <c r="I104" s="4"/>
       <c r="J104" s="5"/>
@@ -4371,20 +4491,20 @@
       <c r="O104" s="5"/>
     </row>
     <row r="105" spans="1:15" ht="18">
-      <c r="A105" s="110"/>
+      <c r="A105" s="113"/>
       <c r="B105" s="1">
         <v>104</v>
       </c>
       <c r="C105" s="16"/>
       <c r="D105" s="37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E105" s="13">
         <v>1</v>
       </c>
-      <c r="F105" s="95"/>
-      <c r="G105" s="95"/>
-      <c r="H105" s="105"/>
+      <c r="F105" s="102"/>
+      <c r="G105" s="102"/>
+      <c r="H105" s="107"/>
       <c r="I105" s="4"/>
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
@@ -4394,7 +4514,7 @@
       <c r="O105" s="5"/>
     </row>
     <row r="106" spans="1:15" ht="18">
-      <c r="A106" s="110"/>
+      <c r="A106" s="113"/>
       <c r="B106" s="1">
         <v>105</v>
       </c>
@@ -4407,9 +4527,9 @@
       <c r="E106" s="13">
         <v>2</v>
       </c>
-      <c r="F106" s="95"/>
-      <c r="G106" s="95"/>
-      <c r="H106" s="105"/>
+      <c r="F106" s="102"/>
+      <c r="G106" s="102"/>
+      <c r="H106" s="107"/>
       <c r="I106" s="4"/>
       <c r="J106" s="5"/>
       <c r="K106" s="5"/>
@@ -4419,7 +4539,7 @@
       <c r="O106" s="5"/>
     </row>
     <row r="107" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A107" s="112"/>
+      <c r="A107" s="117"/>
       <c r="B107" s="1">
         <v>106</v>
       </c>
@@ -4432,9 +4552,9 @@
       <c r="E107" s="13">
         <v>1</v>
       </c>
-      <c r="F107" s="95"/>
-      <c r="G107" s="95"/>
-      <c r="H107" s="105"/>
+      <c r="F107" s="102"/>
+      <c r="G107" s="102"/>
+      <c r="H107" s="107"/>
       <c r="I107" s="4"/>
       <c r="J107" s="5"/>
       <c r="K107" s="5"/>
@@ -4444,7 +4564,7 @@
       <c r="O107" s="5"/>
     </row>
     <row r="108" spans="1:15" ht="18">
-      <c r="A108" s="109" t="s">
+      <c r="A108" s="112" t="s">
         <v>144</v>
       </c>
       <c r="B108" s="1">
@@ -4460,7 +4580,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H108" s="59"/>
       <c r="I108" s="4"/>
@@ -4472,7 +4592,7 @@
       <c r="O108" s="5"/>
     </row>
     <row r="109" spans="1:15" ht="18" customHeight="1">
-      <c r="A109" s="110"/>
+      <c r="A109" s="113"/>
       <c r="B109" s="1">
         <v>108</v>
       </c>
@@ -4486,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H109" s="59"/>
       <c r="I109" s="5"/>
@@ -4498,7 +4618,7 @@
       <c r="O109" s="5"/>
     </row>
     <row r="110" spans="1:15" ht="18">
-      <c r="A110" s="110"/>
+      <c r="A110" s="113"/>
       <c r="B110" s="1">
         <v>109</v>
       </c>
@@ -4512,12 +4632,12 @@
         <v>1</v>
       </c>
       <c r="F110" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H110" s="59"/>
     </row>
     <row r="111" spans="1:15" ht="18.75" thickBot="1">
-      <c r="A111" s="110"/>
+      <c r="A111" s="113"/>
       <c r="B111" s="1">
         <v>110</v>
       </c>
@@ -4531,12 +4651,12 @@
         <v>2</v>
       </c>
       <c r="F111" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H111" s="59"/>
     </row>
     <row r="112" spans="1:15" ht="18">
-      <c r="A112" s="110"/>
+      <c r="A112" s="113"/>
       <c r="B112" s="1">
         <v>111</v>
       </c>
@@ -4550,12 +4670,12 @@
         <v>1</v>
       </c>
       <c r="F112" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H112" s="59"/>
     </row>
     <row r="113" spans="1:8" ht="18">
-      <c r="A113" s="110"/>
+      <c r="A113" s="113"/>
       <c r="B113" s="1">
         <v>112</v>
       </c>
@@ -4569,12 +4689,12 @@
         <v>1</v>
       </c>
       <c r="F113" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H113" s="59"/>
     </row>
     <row r="114" spans="1:8" ht="18">
-      <c r="A114" s="110"/>
+      <c r="A114" s="113"/>
       <c r="B114" s="1">
         <v>113</v>
       </c>
@@ -4588,12 +4708,12 @@
         <v>1</v>
       </c>
       <c r="F114" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H114" s="59"/>
     </row>
     <row r="115" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A115" s="110"/>
+      <c r="A115" s="113"/>
       <c r="B115" s="1">
         <v>114</v>
       </c>
@@ -4605,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="F115" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H115" s="59"/>
     </row>
@@ -4621,7 +4741,7 @@
       <c r="H116" s="59"/>
     </row>
     <row r="117" spans="1:8" ht="18">
-      <c r="A117" s="106" t="s">
+      <c r="A117" s="115" t="s">
         <v>145</v>
       </c>
       <c r="B117" s="1">
@@ -4636,18 +4756,18 @@
       <c r="E117" s="66">
         <v>1</v>
       </c>
-      <c r="F117" s="98" t="s">
-        <v>233</v>
-      </c>
-      <c r="G117" s="98">
+      <c r="F117" s="105" t="s">
+        <v>232</v>
+      </c>
+      <c r="G117" s="105">
         <v>6</v>
       </c>
-      <c r="H117" s="125" t="s">
-        <v>252</v>
+      <c r="H117" s="134" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="18" customHeight="1">
-      <c r="A118" s="107"/>
+      <c r="A118" s="116"/>
       <c r="B118" s="1">
         <v>109</v>
       </c>
@@ -4660,12 +4780,12 @@
       <c r="E118" s="66">
         <v>1</v>
       </c>
-      <c r="F118" s="87"/>
-      <c r="G118" s="87"/>
-      <c r="H118" s="90"/>
+      <c r="F118" s="91"/>
+      <c r="G118" s="91"/>
+      <c r="H118" s="94"/>
     </row>
     <row r="119" spans="1:8" ht="18">
-      <c r="A119" s="107"/>
+      <c r="A119" s="116"/>
       <c r="B119" s="1">
         <v>110</v>
       </c>
@@ -4678,12 +4798,12 @@
       <c r="E119" s="66">
         <v>1</v>
       </c>
-      <c r="F119" s="87"/>
-      <c r="G119" s="87"/>
-      <c r="H119" s="90"/>
+      <c r="F119" s="91"/>
+      <c r="G119" s="91"/>
+      <c r="H119" s="94"/>
     </row>
     <row r="120" spans="1:8" ht="18">
-      <c r="A120" s="107"/>
+      <c r="A120" s="116"/>
       <c r="B120" s="1">
         <v>111</v>
       </c>
@@ -4696,12 +4816,12 @@
       <c r="E120" s="66">
         <v>1</v>
       </c>
-      <c r="F120" s="87"/>
-      <c r="G120" s="87"/>
-      <c r="H120" s="90"/>
+      <c r="F120" s="91"/>
+      <c r="G120" s="91"/>
+      <c r="H120" s="94"/>
     </row>
     <row r="121" spans="1:8" ht="18">
-      <c r="A121" s="107"/>
+      <c r="A121" s="116"/>
       <c r="B121" s="1">
         <v>112</v>
       </c>
@@ -4714,12 +4834,12 @@
       <c r="E121" s="66">
         <v>1</v>
       </c>
-      <c r="F121" s="87"/>
-      <c r="G121" s="87"/>
-      <c r="H121" s="90"/>
+      <c r="F121" s="91"/>
+      <c r="G121" s="91"/>
+      <c r="H121" s="94"/>
     </row>
     <row r="122" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A122" s="107"/>
+      <c r="A122" s="116"/>
       <c r="B122" s="1">
         <v>113</v>
       </c>
@@ -4732,12 +4852,12 @@
       <c r="E122" s="66">
         <v>1</v>
       </c>
-      <c r="F122" s="99"/>
-      <c r="G122" s="99"/>
-      <c r="H122" s="126"/>
+      <c r="F122" s="106"/>
+      <c r="G122" s="106"/>
+      <c r="H122" s="135"/>
     </row>
     <row r="123" spans="1:8" ht="18.75" thickTop="1">
-      <c r="A123" s="107"/>
+      <c r="A123" s="116"/>
       <c r="B123" s="1">
         <v>114</v>
       </c>
@@ -4750,18 +4870,18 @@
       <c r="E123" s="66">
         <v>1</v>
       </c>
-      <c r="F123" s="86" t="s">
-        <v>234</v>
-      </c>
-      <c r="G123" s="86">
+      <c r="F123" s="90" t="s">
+        <v>233</v>
+      </c>
+      <c r="G123" s="90">
         <v>5</v>
       </c>
-      <c r="H123" s="89" t="s">
-        <v>252</v>
+      <c r="H123" s="93" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="18">
-      <c r="A124" s="107"/>
+      <c r="A124" s="116"/>
       <c r="B124" s="1">
         <v>115</v>
       </c>
@@ -4774,12 +4894,12 @@
       <c r="E124" s="66">
         <v>1</v>
       </c>
-      <c r="F124" s="87"/>
-      <c r="G124" s="87"/>
-      <c r="H124" s="90"/>
+      <c r="F124" s="91"/>
+      <c r="G124" s="91"/>
+      <c r="H124" s="94"/>
     </row>
     <row r="125" spans="1:8" ht="18">
-      <c r="A125" s="107"/>
+      <c r="A125" s="116"/>
       <c r="B125" s="1">
         <v>116</v>
       </c>
@@ -4792,12 +4912,12 @@
       <c r="E125" s="66">
         <v>1</v>
       </c>
-      <c r="F125" s="87"/>
-      <c r="G125" s="87"/>
-      <c r="H125" s="90"/>
+      <c r="F125" s="91"/>
+      <c r="G125" s="91"/>
+      <c r="H125" s="94"/>
     </row>
     <row r="126" spans="1:8" ht="18">
-      <c r="A126" s="107"/>
+      <c r="A126" s="116"/>
       <c r="B126" s="1">
         <v>117</v>
       </c>
@@ -4810,12 +4930,12 @@
       <c r="E126" s="66">
         <v>1</v>
       </c>
-      <c r="F126" s="87"/>
-      <c r="G126" s="87"/>
-      <c r="H126" s="90"/>
+      <c r="F126" s="91"/>
+      <c r="G126" s="91"/>
+      <c r="H126" s="94"/>
     </row>
     <row r="127" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A127" s="107"/>
+      <c r="A127" s="116"/>
       <c r="B127" s="1">
         <v>118</v>
       </c>
@@ -4828,9 +4948,9 @@
       <c r="E127" s="82">
         <v>1</v>
       </c>
-      <c r="F127" s="88"/>
-      <c r="G127" s="88"/>
-      <c r="H127" s="91"/>
+      <c r="F127" s="92"/>
+      <c r="G127" s="92"/>
+      <c r="H127" s="95"/>
     </row>
     <row r="128" spans="1:8" ht="18.75" thickTop="1">
       <c r="A128" s="55"/>
@@ -4839,19 +4959,19 @@
         <v>12</v>
       </c>
       <c r="D128" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E128" s="85" t="s">
-        <v>255</v>
-      </c>
-      <c r="F128" s="92" t="s">
-        <v>235</v>
-      </c>
-      <c r="G128" s="92">
+        <v>254</v>
+      </c>
+      <c r="F128" s="96" t="s">
+        <v>234</v>
+      </c>
+      <c r="G128" s="96">
         <v>5</v>
       </c>
-      <c r="H128" s="129" t="s">
-        <v>258</v>
+      <c r="H128" s="99" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="18">
@@ -4861,14 +4981,14 @@
         <v>13</v>
       </c>
       <c r="D129" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E129" s="85" t="s">
-        <v>255</v>
-      </c>
-      <c r="F129" s="93"/>
-      <c r="G129" s="93"/>
-      <c r="H129" s="130"/>
+        <v>254</v>
+      </c>
+      <c r="F129" s="97"/>
+      <c r="G129" s="97"/>
+      <c r="H129" s="100"/>
     </row>
     <row r="130" spans="1:8" ht="18">
       <c r="A130" s="55"/>
@@ -4877,14 +4997,14 @@
         <v>14</v>
       </c>
       <c r="D130" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E130" s="85" t="s">
-        <v>255</v>
-      </c>
-      <c r="F130" s="93"/>
-      <c r="G130" s="93"/>
-      <c r="H130" s="130"/>
+        <v>254</v>
+      </c>
+      <c r="F130" s="97"/>
+      <c r="G130" s="97"/>
+      <c r="H130" s="100"/>
     </row>
     <row r="131" spans="1:8" ht="18">
       <c r="A131" s="55"/>
@@ -4893,14 +5013,14 @@
         <v>15</v>
       </c>
       <c r="D131" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E131" s="85" t="s">
-        <v>255</v>
-      </c>
-      <c r="F131" s="93"/>
-      <c r="G131" s="93"/>
-      <c r="H131" s="130"/>
+        <v>254</v>
+      </c>
+      <c r="F131" s="97"/>
+      <c r="G131" s="97"/>
+      <c r="H131" s="100"/>
     </row>
     <row r="132" spans="1:8" ht="18">
       <c r="A132" s="55"/>
@@ -4909,14 +5029,14 @@
         <v>16</v>
       </c>
       <c r="D132" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E132" s="85" t="s">
-        <v>255</v>
-      </c>
-      <c r="F132" s="94"/>
-      <c r="G132" s="94"/>
-      <c r="H132" s="131"/>
+        <v>254</v>
+      </c>
+      <c r="F132" s="98"/>
+      <c r="G132" s="98"/>
+      <c r="H132" s="101"/>
     </row>
     <row r="133" spans="1:8" ht="18">
       <c r="A133" s="55"/>
@@ -5562,7 +5682,7 @@
       <c r="H196" s="7"/>
     </row>
     <row r="197" spans="1:8" ht="18">
-      <c r="A197" s="111"/>
+      <c r="A197" s="114"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
       <c r="D197" s="4"/>
@@ -5572,7 +5692,7 @@
       <c r="H197" s="7"/>
     </row>
     <row r="198" spans="1:8" ht="18">
-      <c r="A198" s="111"/>
+      <c r="A198" s="114"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
       <c r="D198" s="4"/>
@@ -5580,7 +5700,7 @@
       <c r="F198" s="61"/>
     </row>
     <row r="199" spans="1:8" ht="18">
-      <c r="A199" s="111"/>
+      <c r="A199" s="114"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
       <c r="D199" s="4"/>
@@ -5588,7 +5708,7 @@
       <c r="F199" s="61"/>
     </row>
     <row r="200" spans="1:8" ht="18">
-      <c r="A200" s="111"/>
+      <c r="A200" s="114"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
       <c r="D200" s="4"/>
@@ -5596,7 +5716,7 @@
       <c r="F200" s="61"/>
     </row>
     <row r="201" spans="1:8" ht="18">
-      <c r="A201" s="111"/>
+      <c r="A201" s="114"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
       <c r="D201" s="4"/>
@@ -5604,7 +5724,7 @@
       <c r="F201" s="61"/>
     </row>
     <row r="202" spans="1:8" ht="18">
-      <c r="A202" s="111"/>
+      <c r="A202" s="114"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
       <c r="D202" s="4"/>
@@ -5612,7 +5732,7 @@
       <c r="F202" s="61"/>
     </row>
     <row r="203" spans="1:8" ht="18">
-      <c r="A203" s="111"/>
+      <c r="A203" s="114"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
       <c r="D203" s="4"/>
@@ -5620,7 +5740,7 @@
       <c r="F203" s="61"/>
     </row>
     <row r="204" spans="1:8" ht="18">
-      <c r="A204" s="111"/>
+      <c r="A204" s="114"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
       <c r="D204" s="4"/>
@@ -5628,7 +5748,7 @@
       <c r="F204" s="61"/>
     </row>
     <row r="205" spans="1:8" ht="18">
-      <c r="A205" s="111"/>
+      <c r="A205" s="114"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
       <c r="D205" s="4"/>
@@ -5636,7 +5756,7 @@
       <c r="F205" s="61"/>
     </row>
     <row r="206" spans="1:8" ht="18">
-      <c r="A206" s="111"/>
+      <c r="A206" s="114"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
       <c r="D206" s="4"/>
@@ -5644,7 +5764,7 @@
       <c r="F206" s="61"/>
     </row>
     <row r="207" spans="1:8" ht="18">
-      <c r="A207" s="111"/>
+      <c r="A207" s="114"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
       <c r="D207" s="4"/>
@@ -5652,7 +5772,7 @@
       <c r="F207" s="61"/>
     </row>
     <row r="208" spans="1:8" ht="18">
-      <c r="A208" s="111"/>
+      <c r="A208" s="114"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
       <c r="D208" s="4"/>
@@ -5660,7 +5780,7 @@
       <c r="F208" s="61"/>
     </row>
     <row r="209" spans="1:6" ht="18">
-      <c r="A209" s="111"/>
+      <c r="A209" s="114"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
       <c r="D209" s="4"/>
@@ -5676,7 +5796,7 @@
       <c r="F210" s="61"/>
     </row>
     <row r="211" spans="1:6" ht="18">
-      <c r="A211" s="111"/>
+      <c r="A211" s="114"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
       <c r="D211" s="4"/>
@@ -5684,7 +5804,7 @@
       <c r="F211" s="61"/>
     </row>
     <row r="212" spans="1:6" ht="18">
-      <c r="A212" s="111"/>
+      <c r="A212" s="114"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
       <c r="D212" s="4"/>
@@ -5692,7 +5812,7 @@
       <c r="F212" s="61"/>
     </row>
     <row r="213" spans="1:6" ht="18">
-      <c r="A213" s="111"/>
+      <c r="A213" s="114"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
       <c r="D213" s="4"/>
@@ -5700,7 +5820,7 @@
       <c r="F213" s="61"/>
     </row>
     <row r="214" spans="1:6" ht="18">
-      <c r="A214" s="111"/>
+      <c r="A214" s="114"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
       <c r="D214" s="4"/>
@@ -5708,7 +5828,7 @@
       <c r="F214" s="61"/>
     </row>
     <row r="215" spans="1:6" ht="18">
-      <c r="A215" s="111"/>
+      <c r="A215" s="114"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
       <c r="D215" s="4"/>
@@ -5716,7 +5836,7 @@
       <c r="F215" s="61"/>
     </row>
     <row r="216" spans="1:6" ht="18">
-      <c r="A216" s="111"/>
+      <c r="A216" s="114"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
       <c r="D216" s="4"/>
@@ -5724,7 +5844,7 @@
       <c r="F216" s="61"/>
     </row>
     <row r="217" spans="1:6" ht="18">
-      <c r="A217" s="111"/>
+      <c r="A217" s="114"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
       <c r="D217" s="4"/>
@@ -5732,7 +5852,7 @@
       <c r="F217" s="61"/>
     </row>
     <row r="218" spans="1:6" ht="18">
-      <c r="A218" s="111"/>
+      <c r="A218" s="114"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
       <c r="D218" s="4"/>
@@ -5740,7 +5860,7 @@
       <c r="F218" s="61"/>
     </row>
     <row r="219" spans="1:6" ht="18">
-      <c r="A219" s="111"/>
+      <c r="A219" s="114"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
       <c r="D219" s="4"/>
@@ -5748,7 +5868,7 @@
       <c r="F219" s="61"/>
     </row>
     <row r="220" spans="1:6" ht="18">
-      <c r="A220" s="111"/>
+      <c r="A220" s="114"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
       <c r="D220" s="4"/>
@@ -5756,7 +5876,7 @@
       <c r="F220" s="61"/>
     </row>
     <row r="221" spans="1:6" ht="18">
-      <c r="A221" s="111"/>
+      <c r="A221" s="114"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
       <c r="D221" s="4"/>
@@ -5764,7 +5884,7 @@
       <c r="F221" s="61"/>
     </row>
     <row r="222" spans="1:6" ht="18">
-      <c r="A222" s="111"/>
+      <c r="A222" s="114"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
       <c r="D222" s="4"/>
@@ -5772,7 +5892,7 @@
       <c r="F222" s="61"/>
     </row>
     <row r="223" spans="1:6" ht="18">
-      <c r="A223" s="111"/>
+      <c r="A223" s="114"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="4"/>
@@ -5780,7 +5900,7 @@
       <c r="F223" s="61"/>
     </row>
     <row r="224" spans="1:6" ht="18">
-      <c r="A224" s="111"/>
+      <c r="A224" s="114"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
       <c r="D224" s="4"/>
@@ -5788,7 +5908,7 @@
       <c r="F224" s="61"/>
     </row>
     <row r="225" spans="1:6" ht="18">
-      <c r="A225" s="111"/>
+      <c r="A225" s="114"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
       <c r="D225" s="4"/>
@@ -5796,7 +5916,7 @@
       <c r="F225" s="61"/>
     </row>
     <row r="226" spans="1:6" ht="18">
-      <c r="A226" s="111"/>
+      <c r="A226" s="114"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
       <c r="D226" s="4"/>
@@ -5804,7 +5924,7 @@
       <c r="F226" s="61"/>
     </row>
     <row r="227" spans="1:6" ht="18">
-      <c r="A227" s="111"/>
+      <c r="A227" s="114"/>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
       <c r="D227" s="4"/>
@@ -5812,7 +5932,7 @@
       <c r="F227" s="61"/>
     </row>
     <row r="228" spans="1:6" ht="18">
-      <c r="A228" s="111"/>
+      <c r="A228" s="114"/>
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
       <c r="D228" s="4"/>
@@ -5820,7 +5940,7 @@
       <c r="F228" s="61"/>
     </row>
     <row r="229" spans="1:6" ht="18">
-      <c r="A229" s="111"/>
+      <c r="A229" s="114"/>
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
       <c r="D229" s="4"/>
@@ -5828,7 +5948,7 @@
       <c r="F229" s="61"/>
     </row>
     <row r="230" spans="1:6" ht="18">
-      <c r="A230" s="111"/>
+      <c r="A230" s="114"/>
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
       <c r="D230" s="4"/>
@@ -5836,7 +5956,7 @@
       <c r="F230" s="61"/>
     </row>
     <row r="231" spans="1:6" ht="18">
-      <c r="A231" s="111"/>
+      <c r="A231" s="114"/>
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
       <c r="D231" s="4"/>
@@ -5844,7 +5964,7 @@
       <c r="F231" s="61"/>
     </row>
     <row r="232" spans="1:6" ht="18">
-      <c r="A232" s="111"/>
+      <c r="A232" s="114"/>
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
       <c r="D232" s="4"/>
@@ -5852,7 +5972,7 @@
       <c r="F232" s="61"/>
     </row>
     <row r="233" spans="1:6" ht="18">
-      <c r="A233" s="111"/>
+      <c r="A233" s="114"/>
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
       <c r="D233" s="4"/>
@@ -5860,7 +5980,7 @@
       <c r="F233" s="61"/>
     </row>
     <row r="234" spans="1:6" ht="18">
-      <c r="A234" s="111"/>
+      <c r="A234" s="114"/>
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
       <c r="D234" s="4"/>
@@ -5868,7 +5988,7 @@
       <c r="F234" s="61"/>
     </row>
     <row r="235" spans="1:6" ht="18">
-      <c r="A235" s="111"/>
+      <c r="A235" s="114"/>
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
       <c r="D235" s="4"/>
@@ -5930,9 +6050,7 @@
     <mergeCell ref="H59:H62"/>
     <mergeCell ref="H67:H70"/>
     <mergeCell ref="H71:H74"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="H63:H66"/>
     <mergeCell ref="H47:H50"/>
     <mergeCell ref="H51:H53"/>
     <mergeCell ref="H54:H56"/>
@@ -5963,6 +6081,17 @@
     <mergeCell ref="G33:G36"/>
     <mergeCell ref="G37:G40"/>
     <mergeCell ref="A29:A46"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="H37:H40"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H43:H46"/>
     <mergeCell ref="A108:A115"/>
     <mergeCell ref="A197:A209"/>
     <mergeCell ref="A211:A235"/>
@@ -5979,23 +6108,14 @@
     <mergeCell ref="F79:F81"/>
     <mergeCell ref="F84:F86"/>
     <mergeCell ref="F91:F93"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="H33:H36"/>
     <mergeCell ref="G57:G58"/>
     <mergeCell ref="G75:G78"/>
     <mergeCell ref="G79:G81"/>
     <mergeCell ref="G82:G83"/>
     <mergeCell ref="G84:G86"/>
-    <mergeCell ref="H63:H66"/>
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F41:F42"/>
     <mergeCell ref="F57:F58"/>
     <mergeCell ref="F82:F83"/>
     <mergeCell ref="F94:F95"/>
@@ -6044,170 +6164,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F25"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="42" t="s">
+      <c r="C1" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="86" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="C2" s="136" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="136">
+        <v>8</v>
+      </c>
+      <c r="E2" s="136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A4" s="43" t="s">
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+    </row>
+    <row r="4" spans="1:5" ht="18">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="53" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A5" s="44" t="s">
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+    </row>
+    <row r="8" spans="1:5" ht="18">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="137"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+    </row>
+    <row r="9" spans="1:5" ht="18">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+    </row>
+    <row r="10" spans="1:5" ht="18">
+      <c r="B10" s="88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18">
+      <c r="B11" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18">
+      <c r="B12" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" thickBot="1">
+      <c r="B13" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18">
+      <c r="B14" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18">
+      <c r="B15" s="43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18">
+      <c r="B16" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B17" s="44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="18">
+      <c r="B18" s="42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="18">
+      <c r="B19" s="43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="18">
+      <c r="B20" s="43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B21" s="44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="18">
+      <c r="B22" s="42" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18">
-      <c r="A6" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="43" t="s">
+    <row r="23" spans="2:2" ht="18">
+      <c r="B23" s="43" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18">
-      <c r="A7" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="43" t="s">
+    <row r="24" spans="2:2" ht="18">
+      <c r="B24" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A8" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="44" t="s">
+    <row r="25" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B25" s="44" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A9" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="42" t="s">
+    <row r="26" spans="2:2" ht="18">
+      <c r="B26" s="42" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18">
-      <c r="A10" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="43" t="s">
+    <row r="27" spans="2:2" ht="18">
+      <c r="B27" s="43" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A11" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="44" t="s">
+    <row r="28" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B28" s="44" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18">
-      <c r="A12" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="42" t="s">
+    <row r="29" spans="2:2" ht="18">
+      <c r="B29" s="42" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A13" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="43" t="s">
+    <row r="30" spans="2:2" ht="18">
+      <c r="B30" s="43" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A14" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="44" t="s">
+    <row r="31" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B31" s="44" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18">
-      <c r="A15" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="42" t="s">
+    <row r="32" spans="2:2" ht="18">
+      <c r="B32" s="42" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18">
-      <c r="A16" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="43" t="s">
+    <row r="33" spans="2:2" ht="18">
+      <c r="B33" s="43" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A17" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="43" t="s">
+    <row r="34" spans="2:2" ht="18">
+      <c r="B34" s="43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A18" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="47" t="s">
+    <row r="35" spans="2:2" ht="18.75" thickBot="1">
+      <c r="B35" s="47" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18">
-      <c r="A19" s="43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18">
-      <c r="A20" s="43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" thickBot="1">
-      <c r="A21" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6274,13 +6491,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="9"/>
       <c r="B8" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75">
@@ -6413,122 +6630,122 @@
     </row>
     <row r="2" spans="1:1" ht="18">
       <c r="A2" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18">
       <c r="A3" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18">
       <c r="A4" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18">
       <c r="A5" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18">
       <c r="A6" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18">
       <c r="A7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18">
       <c r="A8" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18">
       <c r="A9" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18">
       <c r="A10" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18">
       <c r="A11" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18">
       <c r="A12" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18">
       <c r="A13" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18">
       <c r="A14" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18">
       <c r="A15" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18">
       <c r="A16" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18">
       <c r="A17" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18">
       <c r="A18" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18">
       <c r="A19" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18">
       <c r="A20" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18">
       <c r="A21" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18">
       <c r="A22" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18">
       <c r="A23" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18">
       <c r="A24" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18">
       <c r="A25" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18">
@@ -6551,32 +6768,32 @@
     </row>
     <row r="39" spans="1:1" ht="18">
       <c r="A39" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18">
       <c r="A40" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="18">
       <c r="A41" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="18">
       <c r="A42" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18">
       <c r="A43" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18">
       <c r="A44" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -6586,4 +6803,139 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" thickBot="1">
+      <c r="A1" s="143" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="143" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5" thickTop="1">
+      <c r="A2" s="138" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="141" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="141"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="139" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="139"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="139"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="139"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="139"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="139"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="138" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="139" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14" s="139"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="139"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="139"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="140" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="142" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>